<commit_message>
Tekst usklađen sa 110000 verzijom zakrpe
</commit_message>
<xml_diff>
--- a/Fajlovi za pomoć/Imena u StalkerSoup-u.xlsx
+++ b/Fajlovi za pomoć/Imena u StalkerSoup-u.xlsx
@@ -1910,7 +1910,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="455">
   <si>
     <t>B.R.</t>
   </si>
@@ -2128,9 +2128,6 @@
     <t xml:space="preserve">Forgotten Forest </t>
   </si>
   <si>
-    <t>Crest</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cave </t>
   </si>
   <si>
@@ -3115,9 +3112,6 @@
     <t>Igrač</t>
   </si>
   <si>
-    <t>Marked</t>
-  </si>
-  <si>
     <t>Obeleženi</t>
   </si>
   <si>
@@ -3266,6 +3260,21 @@
   </si>
   <si>
     <t>Škrti</t>
+  </si>
+  <si>
+    <t>Crest ili Cross</t>
+  </si>
+  <si>
+    <t>Marked One</t>
+  </si>
+  <si>
+    <t>Caesier</t>
+  </si>
+  <si>
+    <t>Cezar</t>
+  </si>
+  <si>
+    <t>Kolektor - igra</t>
   </si>
 </sst>
 </file>
@@ -3891,10 +3900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M196"/>
+  <dimension ref="A2:M198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="L96" sqref="L96:M96"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,7 +3926,7 @@
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" s="26" t="s">
@@ -3925,15 +3934,15 @@
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I2" s="26"/>
       <c r="J2" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K2" s="26"/>
       <c r="L2" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M2" s="19"/>
     </row>
@@ -3957,19 +3966,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13" t="s">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="13"/>
@@ -4002,7 +4011,7 @@
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="17" t="s">
@@ -4028,7 +4037,7 @@
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="17" t="s">
@@ -4036,7 +4045,7 @@
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="7"/>
@@ -4054,7 +4063,7 @@
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="17" t="s">
@@ -4062,7 +4071,7 @@
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="7"/>
@@ -4080,7 +4089,7 @@
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="17" t="s">
@@ -4088,7 +4097,7 @@
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="7"/>
@@ -4106,7 +4115,7 @@
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="17" t="s">
@@ -4114,7 +4123,7 @@
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="7"/>
@@ -4132,7 +4141,7 @@
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="17" t="s">
@@ -4158,7 +4167,7 @@
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="17" t="s">
@@ -4166,11 +4175,11 @@
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -4186,7 +4195,7 @@
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="17" t="s">
@@ -4194,7 +4203,7 @@
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I13" s="18"/>
       <c r="J13" s="7"/>
@@ -4212,7 +4221,7 @@
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="17" t="s">
@@ -4220,7 +4229,7 @@
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I14" s="18"/>
       <c r="J14" s="7"/>
@@ -4238,15 +4247,15 @@
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I15" s="18"/>
       <c r="J15" s="17"/>
@@ -4264,15 +4273,15 @@
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E16" s="21"/>
       <c r="F16" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="17"/>
@@ -4290,15 +4299,15 @@
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I17" s="18"/>
       <c r="J17" s="17"/>
@@ -4316,15 +4325,15 @@
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I18" s="18"/>
       <c r="J18" s="17"/>
@@ -4342,19 +4351,19 @@
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="17" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K19" s="18"/>
       <c r="L19" s="7"/>
@@ -4370,15 +4379,15 @@
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I20" s="18"/>
       <c r="J20" s="17"/>
@@ -4396,19 +4405,19 @@
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I21" s="18"/>
       <c r="J21" s="17" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K21" s="18"/>
       <c r="L21" s="7"/>
@@ -4424,15 +4433,15 @@
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="17"/>
@@ -4450,15 +4459,15 @@
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G23" s="18"/>
       <c r="H23" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I23" s="18"/>
       <c r="J23" s="17"/>
@@ -4487,11 +4496,11 @@
         <v>20</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="17" t="s">
@@ -4499,7 +4508,7 @@
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="7"/>
@@ -4513,11 +4522,11 @@
         <v>21</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="17" t="s">
@@ -4539,11 +4548,11 @@
         <v>22</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="17" t="s">
@@ -4551,11 +4560,11 @@
       </c>
       <c r="G27" s="18"/>
       <c r="H27" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
@@ -4567,11 +4576,11 @@
         <v>23</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="17" t="s">
@@ -4579,7 +4588,7 @@
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="7"/>
@@ -4593,11 +4602,11 @@
         <v>24</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="17" t="s">
@@ -4605,7 +4614,7 @@
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="7"/>
@@ -4619,11 +4628,11 @@
         <v>25</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="17" t="s">
@@ -4631,11 +4640,11 @@
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I30" s="18"/>
       <c r="J30" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
@@ -4647,11 +4656,11 @@
         <v>26</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="17" t="s">
@@ -4659,7 +4668,7 @@
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I31" s="18"/>
       <c r="J31" s="7"/>
@@ -4673,11 +4682,11 @@
         <v>27</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="17" t="s">
@@ -4685,7 +4694,7 @@
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I32" s="18"/>
       <c r="J32" s="7"/>
@@ -4699,11 +4708,11 @@
         <v>28</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="17" t="s">
@@ -4711,11 +4720,11 @@
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I33" s="18"/>
       <c r="J33" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
@@ -4727,7 +4736,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="17" t="s">
@@ -4739,11 +4748,11 @@
       </c>
       <c r="G34" s="18"/>
       <c r="H34" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I34" s="18"/>
       <c r="J34" s="7" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
@@ -4755,11 +4764,11 @@
         <v>30</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="17" t="s">
@@ -4767,7 +4776,7 @@
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I35" s="18"/>
       <c r="J35" s="7"/>
@@ -4781,19 +4790,19 @@
         <v>31</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E36" s="25"/>
       <c r="F36" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="7"/>
@@ -4807,19 +4816,19 @@
         <v>32</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="7"/>
@@ -4833,19 +4842,19 @@
         <v>33</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I38" s="18"/>
       <c r="J38" s="7"/>
@@ -4859,19 +4868,19 @@
         <v>34</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E39" s="25"/>
       <c r="F39" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I39" s="18"/>
       <c r="J39" s="7"/>
@@ -4904,7 +4913,7 @@
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="17" t="s">
@@ -4930,7 +4939,7 @@
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="17" t="s">
@@ -4938,7 +4947,7 @@
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I42" s="18"/>
       <c r="J42" s="7"/>
@@ -4956,19 +4965,19 @@
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E43" s="18"/>
       <c r="F43" s="17" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G43" s="18"/>
       <c r="H43" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I43" s="18"/>
       <c r="J43" s="7" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
@@ -4984,7 +4993,7 @@
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E44" s="18"/>
       <c r="F44" s="17" t="s">
@@ -4992,7 +5001,7 @@
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I44" s="18"/>
       <c r="J44" s="7"/>
@@ -5010,19 +5019,19 @@
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G45" s="18"/>
       <c r="H45" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I45" s="18"/>
       <c r="J45" s="7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
@@ -5038,15 +5047,15 @@
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E46" s="18"/>
       <c r="F46" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G46" s="18"/>
       <c r="H46" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I46" s="18"/>
       <c r="J46" s="7"/>
@@ -5064,15 +5073,15 @@
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E47" s="18"/>
       <c r="F47" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I47" s="18"/>
       <c r="J47" s="7"/>
@@ -5090,19 +5099,19 @@
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E48" s="25"/>
       <c r="F48" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I48" s="18"/>
       <c r="J48" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
@@ -5133,15 +5142,15 @@
       </c>
       <c r="C50" s="18"/>
       <c r="D50" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G50" s="18"/>
       <c r="H50" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I50" s="18"/>
       <c r="J50" s="7"/>
@@ -5159,7 +5168,7 @@
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E51" s="21"/>
       <c r="F51" s="17" t="s">
@@ -5167,7 +5176,7 @@
       </c>
       <c r="G51" s="18"/>
       <c r="H51" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I51" s="18"/>
       <c r="J51" s="7"/>
@@ -5185,7 +5194,7 @@
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="17" t="s">
@@ -5193,7 +5202,7 @@
       </c>
       <c r="G52" s="18"/>
       <c r="H52" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I52" s="18"/>
       <c r="J52" s="7"/>
@@ -5211,7 +5220,7 @@
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E53" s="18"/>
       <c r="F53" s="17" t="s">
@@ -5237,15 +5246,15 @@
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E54" s="18"/>
       <c r="F54" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G54" s="18"/>
       <c r="H54" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I54" s="18"/>
       <c r="J54" s="7"/>
@@ -5263,7 +5272,7 @@
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E55" s="18"/>
       <c r="F55" s="17" t="s">
@@ -5271,7 +5280,7 @@
       </c>
       <c r="G55" s="18"/>
       <c r="H55" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I55" s="18"/>
       <c r="J55" s="7"/>
@@ -5289,15 +5298,15 @@
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E56" s="18"/>
       <c r="F56" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G56" s="18"/>
       <c r="H56" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I56" s="18"/>
       <c r="J56" s="7"/>
@@ -5315,15 +5324,15 @@
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E57" s="21"/>
       <c r="F57" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G57" s="18"/>
       <c r="H57" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I57" s="18"/>
       <c r="J57" s="7"/>
@@ -5341,15 +5350,15 @@
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E58" s="18"/>
       <c r="F58" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G58" s="18"/>
       <c r="H58" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I58" s="18"/>
       <c r="J58" s="7"/>
@@ -5367,15 +5376,15 @@
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E59" s="18"/>
       <c r="F59" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G59" s="18"/>
       <c r="H59" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I59" s="18"/>
       <c r="J59" s="7"/>
@@ -5408,15 +5417,15 @@
       </c>
       <c r="C61" s="18"/>
       <c r="D61" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E61" s="18"/>
       <c r="F61" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G61" s="18"/>
       <c r="H61" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I61" s="18"/>
       <c r="J61" s="7"/>
@@ -5434,7 +5443,7 @@
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="17" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E62" s="18"/>
       <c r="F62" s="17" t="s">
@@ -5442,7 +5451,7 @@
       </c>
       <c r="G62" s="18"/>
       <c r="H62" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I62" s="18"/>
       <c r="J62" s="7"/>
@@ -5460,7 +5469,7 @@
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E63" s="18"/>
       <c r="F63" s="17" t="s">
@@ -5468,7 +5477,7 @@
       </c>
       <c r="G63" s="18"/>
       <c r="H63" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I63" s="18"/>
       <c r="J63" s="7"/>
@@ -5486,15 +5495,15 @@
       </c>
       <c r="C64" s="18"/>
       <c r="D64" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E64" s="18"/>
       <c r="F64" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G64" s="18"/>
       <c r="H64" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I64" s="18"/>
       <c r="J64" s="7"/>
@@ -5512,15 +5521,15 @@
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E65" s="21"/>
       <c r="F65" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G65" s="18"/>
       <c r="H65" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I65" s="18"/>
       <c r="J65" s="7"/>
@@ -5538,15 +5547,15 @@
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E66" s="23"/>
       <c r="F66" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G66" s="18"/>
       <c r="H66" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I66" s="18"/>
       <c r="J66" s="7"/>
@@ -5564,15 +5573,15 @@
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E67" s="18"/>
       <c r="F67" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G67" s="18"/>
       <c r="H67" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I67" s="18"/>
       <c r="J67" s="7"/>
@@ -5590,15 +5599,15 @@
       </c>
       <c r="C68" s="18"/>
       <c r="D68" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E68" s="18"/>
       <c r="F68" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G68" s="18"/>
       <c r="H68" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I68" s="18"/>
       <c r="J68" s="7"/>
@@ -5631,7 +5640,7 @@
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E70" s="18"/>
       <c r="F70" s="17" t="s">
@@ -5657,7 +5666,7 @@
       </c>
       <c r="C71" s="18"/>
       <c r="D71" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E71" s="18"/>
       <c r="F71" s="17" t="s">
@@ -5665,11 +5674,11 @@
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I71" s="18"/>
       <c r="J71" s="7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
@@ -5685,7 +5694,7 @@
       </c>
       <c r="C72" s="18"/>
       <c r="D72" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E72" s="18"/>
       <c r="F72" s="17" t="s">
@@ -5693,7 +5702,7 @@
       </c>
       <c r="G72" s="18"/>
       <c r="H72" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I72" s="18"/>
       <c r="J72" s="7"/>
@@ -5711,7 +5720,7 @@
       </c>
       <c r="C73" s="18"/>
       <c r="D73" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E73" s="18"/>
       <c r="F73" s="17" t="s">
@@ -5737,7 +5746,7 @@
       </c>
       <c r="C74" s="18"/>
       <c r="D74" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E74" s="21"/>
       <c r="F74" s="17" t="s">
@@ -5745,7 +5754,7 @@
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I74" s="18"/>
       <c r="J74" s="7"/>
@@ -5771,7 +5780,7 @@
       </c>
       <c r="G75" s="18"/>
       <c r="H75" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I75" s="18"/>
       <c r="J75" s="7"/>
@@ -5789,7 +5798,7 @@
       </c>
       <c r="C76" s="18"/>
       <c r="D76" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E76" s="21"/>
       <c r="F76" s="17" t="s">
@@ -5797,7 +5806,7 @@
       </c>
       <c r="G76" s="18"/>
       <c r="H76" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I76" s="18"/>
       <c r="J76" s="7"/>
@@ -5815,7 +5824,7 @@
       </c>
       <c r="C77" s="18"/>
       <c r="D77" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E77" s="18"/>
       <c r="F77" s="17" t="s">
@@ -5823,7 +5832,7 @@
       </c>
       <c r="G77" s="18"/>
       <c r="H77" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I77" s="18"/>
       <c r="J77" s="7"/>
@@ -5841,7 +5850,7 @@
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E78" s="18"/>
       <c r="F78" s="17" t="s">
@@ -5849,7 +5858,7 @@
       </c>
       <c r="G78" s="18"/>
       <c r="H78" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I78" s="18"/>
       <c r="J78" s="7"/>
@@ -5867,15 +5876,15 @@
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E79" s="18"/>
       <c r="F79" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G79" s="18"/>
       <c r="H79" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I79" s="18"/>
       <c r="J79" s="7"/>
@@ -5893,7 +5902,7 @@
       </c>
       <c r="C80" s="18"/>
       <c r="D80" s="17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E80" s="18"/>
       <c r="F80" s="17" t="s">
@@ -5901,7 +5910,7 @@
       </c>
       <c r="G80" s="18"/>
       <c r="H80" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I80" s="18"/>
       <c r="J80" s="7"/>
@@ -5919,19 +5928,19 @@
       </c>
       <c r="C81" s="18"/>
       <c r="D81" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E81" s="18"/>
       <c r="F81" s="17" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G81" s="18"/>
       <c r="H81" s="17" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I81" s="18"/>
       <c r="J81" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
@@ -5955,11 +5964,11 @@
       </c>
       <c r="G82" s="18"/>
       <c r="H82" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I82" s="18"/>
       <c r="J82" s="17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="K82" s="18"/>
       <c r="L82" s="7"/>
@@ -5975,7 +5984,7 @@
       </c>
       <c r="C83" s="18"/>
       <c r="D83" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E83" s="21"/>
       <c r="F83" s="17" t="s">
@@ -5983,7 +5992,7 @@
       </c>
       <c r="G83" s="18"/>
       <c r="H83" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I83" s="18"/>
       <c r="J83" s="7"/>
@@ -6001,15 +6010,15 @@
       </c>
       <c r="C84" s="18"/>
       <c r="D84" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E84" s="25"/>
       <c r="F84" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G84" s="18"/>
       <c r="H84" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I84" s="18"/>
       <c r="J84" s="7"/>
@@ -6027,15 +6036,15 @@
       </c>
       <c r="C85" s="18"/>
       <c r="D85" s="17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E85" s="18"/>
       <c r="F85" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G85" s="18"/>
       <c r="H85" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I85" s="18"/>
       <c r="J85" s="7"/>
@@ -6053,15 +6062,15 @@
       </c>
       <c r="C86" s="18"/>
       <c r="D86" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E86" s="21"/>
       <c r="F86" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G86" s="18"/>
       <c r="H86" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I86" s="18"/>
       <c r="J86" s="7"/>
@@ -6090,19 +6099,19 @@
         <v>78</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C88" s="14"/>
       <c r="D88" s="13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E88" s="14"/>
       <c r="F88" s="13" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G88" s="14"/>
       <c r="H88" s="13" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I88" s="14"/>
       <c r="J88" s="13"/>
@@ -6116,19 +6125,19 @@
         <v>79</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C89" s="14"/>
       <c r="D89" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E89" s="14"/>
       <c r="F89" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G89" s="14"/>
       <c r="H89" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I89" s="14"/>
       <c r="J89" s="13"/>
@@ -6161,7 +6170,7 @@
       </c>
       <c r="C91" s="18"/>
       <c r="D91" s="17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E91" s="18"/>
       <c r="F91" s="17" t="s">
@@ -6169,7 +6178,7 @@
       </c>
       <c r="G91" s="18"/>
       <c r="H91" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I91" s="18"/>
       <c r="J91" s="7"/>
@@ -6187,7 +6196,7 @@
       </c>
       <c r="C92" s="18"/>
       <c r="D92" s="17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E92" s="18"/>
       <c r="F92" s="17" t="s">
@@ -6195,7 +6204,7 @@
       </c>
       <c r="G92" s="18"/>
       <c r="H92" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I92" s="18"/>
       <c r="J92" s="7"/>
@@ -6219,7 +6228,7 @@
       </c>
       <c r="G93" s="18"/>
       <c r="H93" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I93" s="18"/>
       <c r="J93" s="7"/>
@@ -6237,7 +6246,7 @@
       </c>
       <c r="C94" s="18"/>
       <c r="D94" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E94" s="18"/>
       <c r="F94" s="17" t="s">
@@ -6245,7 +6254,7 @@
       </c>
       <c r="G94" s="18"/>
       <c r="H94" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I94" s="18"/>
       <c r="J94" s="7"/>
@@ -6263,15 +6272,15 @@
       </c>
       <c r="C95" s="18"/>
       <c r="D95" s="17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E95" s="18"/>
       <c r="F95" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G95" s="18"/>
       <c r="H95" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I95" s="18"/>
       <c r="J95" s="7"/>
@@ -6289,7 +6298,7 @@
       </c>
       <c r="C96" s="18"/>
       <c r="D96" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E96" s="18"/>
       <c r="F96" s="17" t="s">
@@ -6297,15 +6306,15 @@
       </c>
       <c r="G96" s="18"/>
       <c r="H96" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I96" s="18"/>
       <c r="J96" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K96" s="7"/>
       <c r="L96" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="M96" s="7"/>
     </row>
@@ -6319,15 +6328,15 @@
       </c>
       <c r="C97" s="18"/>
       <c r="D97" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E97" s="21"/>
       <c r="F97" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G97" s="18"/>
       <c r="H97" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I97" s="18"/>
       <c r="J97" s="7"/>
@@ -6345,15 +6354,15 @@
       </c>
       <c r="C98" s="18"/>
       <c r="D98" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E98" s="23"/>
       <c r="F98" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G98" s="18"/>
       <c r="H98" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I98" s="18"/>
       <c r="J98" s="7"/>
@@ -6371,15 +6380,15 @@
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E99" s="21"/>
       <c r="F99" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G99" s="18"/>
       <c r="H99" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I99" s="18"/>
       <c r="J99" s="7"/>
@@ -6397,15 +6406,15 @@
       </c>
       <c r="C100" s="18"/>
       <c r="D100" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E100" s="21"/>
       <c r="F100" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G100" s="18"/>
       <c r="H100" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I100" s="18"/>
       <c r="J100" s="7"/>
@@ -6423,15 +6432,15 @@
       </c>
       <c r="C101" s="18"/>
       <c r="D101" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E101" s="18"/>
       <c r="F101" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G101" s="18"/>
       <c r="H101" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I101" s="18"/>
       <c r="J101" s="7"/>
@@ -6449,15 +6458,15 @@
       </c>
       <c r="C102" s="18"/>
       <c r="D102" s="17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E102" s="18"/>
       <c r="F102" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G102" s="18"/>
       <c r="H102" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I102" s="18"/>
       <c r="J102" s="7"/>
@@ -6475,15 +6484,15 @@
       </c>
       <c r="C103" s="18"/>
       <c r="D103" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E103" s="18"/>
       <c r="F103" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G103" s="18"/>
       <c r="H103" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I103" s="18"/>
       <c r="J103" s="7"/>
@@ -6501,15 +6510,15 @@
       </c>
       <c r="C104" s="18"/>
       <c r="D104" s="17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E104" s="18"/>
       <c r="F104" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G104" s="18"/>
       <c r="H104" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I104" s="18"/>
       <c r="J104" s="7"/>
@@ -6529,11 +6538,11 @@
       <c r="D105" s="17"/>
       <c r="E105" s="18"/>
       <c r="F105" s="17" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G105" s="18"/>
       <c r="H105" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I105" s="18"/>
       <c r="J105" s="7"/>
@@ -6566,7 +6575,7 @@
       </c>
       <c r="C107" s="18"/>
       <c r="D107" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E107" s="18"/>
       <c r="F107" s="17" t="s">
@@ -6574,7 +6583,7 @@
       </c>
       <c r="G107" s="18"/>
       <c r="H107" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I107" s="18"/>
       <c r="J107" s="7"/>
@@ -6592,7 +6601,7 @@
       </c>
       <c r="C108" s="18"/>
       <c r="D108" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E108" s="23"/>
       <c r="F108" s="17" t="s">
@@ -6600,7 +6609,7 @@
       </c>
       <c r="G108" s="18"/>
       <c r="H108" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I108" s="18"/>
       <c r="J108" s="7"/>
@@ -6618,19 +6627,19 @@
       </c>
       <c r="C109" s="18"/>
       <c r="D109" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E109" s="18"/>
       <c r="F109" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G109" s="18"/>
       <c r="H109" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I109" s="18"/>
       <c r="J109" s="7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K109" s="7"/>
       <c r="L109" s="7"/>
@@ -6661,15 +6670,15 @@
       </c>
       <c r="C111" s="18"/>
       <c r="D111" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E111" s="18"/>
       <c r="F111" s="17" t="s">
-        <v>72</v>
+        <v>450</v>
       </c>
       <c r="G111" s="18"/>
       <c r="H111" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I111" s="18"/>
       <c r="J111" s="7"/>
@@ -6702,7 +6711,7 @@
       </c>
       <c r="C113" s="18"/>
       <c r="D113" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E113" s="18"/>
       <c r="F113" s="17" t="s">
@@ -6710,7 +6719,7 @@
       </c>
       <c r="G113" s="18"/>
       <c r="H113" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I113" s="18"/>
       <c r="J113" s="7"/>
@@ -6728,7 +6737,7 @@
       </c>
       <c r="C114" s="18"/>
       <c r="D114" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E114" s="18"/>
       <c r="F114" s="17" t="s">
@@ -6736,11 +6745,11 @@
       </c>
       <c r="G114" s="18"/>
       <c r="H114" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I114" s="18"/>
       <c r="J114" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K114" s="7"/>
       <c r="L114" s="7"/>
@@ -6756,7 +6765,7 @@
       </c>
       <c r="C115" s="18"/>
       <c r="D115" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E115" s="18"/>
       <c r="F115" s="17" t="s">
@@ -6764,11 +6773,11 @@
       </c>
       <c r="G115" s="18"/>
       <c r="H115" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I115" s="18"/>
       <c r="J115" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K115" s="7"/>
       <c r="L115" s="7"/>
@@ -6799,7 +6808,7 @@
       </c>
       <c r="C117" s="18"/>
       <c r="D117" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E117" s="23"/>
       <c r="F117" s="17" t="s">
@@ -6807,7 +6816,7 @@
       </c>
       <c r="G117" s="18"/>
       <c r="H117" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I117" s="18"/>
       <c r="J117" s="7"/>
@@ -6825,15 +6834,15 @@
       </c>
       <c r="C118" s="18"/>
       <c r="D118" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E118" s="18"/>
       <c r="F118" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G118" s="18"/>
       <c r="H118" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I118" s="18"/>
       <c r="J118" s="7"/>
@@ -6851,15 +6860,15 @@
       </c>
       <c r="C119" s="18"/>
       <c r="D119" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E119" s="18"/>
       <c r="F119" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G119" s="18"/>
       <c r="H119" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I119" s="18"/>
       <c r="J119" s="7"/>
@@ -6877,15 +6886,15 @@
       </c>
       <c r="C120" s="18"/>
       <c r="D120" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E120" s="18"/>
       <c r="F120" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G120" s="18"/>
       <c r="H120" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I120" s="18"/>
       <c r="J120" s="7"/>
@@ -6903,15 +6912,15 @@
       </c>
       <c r="C121" s="18"/>
       <c r="D121" s="17" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E121" s="18"/>
       <c r="F121" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G121" s="18"/>
       <c r="H121" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I121" s="18"/>
       <c r="J121" s="7"/>
@@ -6944,7 +6953,7 @@
       </c>
       <c r="C123" s="18"/>
       <c r="D123" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E123" s="18"/>
       <c r="F123" s="17" t="s">
@@ -6952,7 +6961,7 @@
       </c>
       <c r="G123" s="18"/>
       <c r="H123" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I123" s="18"/>
       <c r="J123" s="7"/>
@@ -6970,7 +6979,7 @@
       </c>
       <c r="C124" s="18"/>
       <c r="D124" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E124" s="18"/>
       <c r="F124" s="17" t="s">
@@ -6978,7 +6987,7 @@
       </c>
       <c r="G124" s="18"/>
       <c r="H124" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I124" s="18"/>
       <c r="J124" s="7"/>
@@ -6996,7 +7005,7 @@
       </c>
       <c r="C125" s="18"/>
       <c r="D125" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E125" s="18"/>
       <c r="F125" s="17" t="s">
@@ -7004,7 +7013,7 @@
       </c>
       <c r="G125" s="18"/>
       <c r="H125" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I125" s="18"/>
       <c r="J125" s="7"/>
@@ -7022,7 +7031,7 @@
       </c>
       <c r="C126" s="18"/>
       <c r="D126" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E126" s="18"/>
       <c r="F126" s="17" t="s">
@@ -7030,7 +7039,7 @@
       </c>
       <c r="G126" s="18"/>
       <c r="H126" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I126" s="18"/>
       <c r="J126" s="7"/>
@@ -7048,15 +7057,15 @@
       </c>
       <c r="C127" s="18"/>
       <c r="D127" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E127" s="18"/>
       <c r="F127" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G127" s="18"/>
       <c r="H127" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I127" s="18"/>
       <c r="J127" s="7"/>
@@ -7074,15 +7083,15 @@
       </c>
       <c r="C128" s="18"/>
       <c r="D128" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E128" s="25"/>
       <c r="F128" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G128" s="18"/>
       <c r="H128" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I128" s="18"/>
       <c r="J128" s="7"/>
@@ -7100,15 +7109,15 @@
       </c>
       <c r="C129" s="18"/>
       <c r="D129" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E129" s="18"/>
       <c r="F129" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G129" s="18"/>
       <c r="H129" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I129" s="18"/>
       <c r="J129" s="7"/>
@@ -7126,15 +7135,15 @@
       </c>
       <c r="C130" s="18"/>
       <c r="D130" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E130" s="23"/>
       <c r="F130" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G130" s="18"/>
       <c r="H130" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I130" s="18"/>
       <c r="J130" s="7"/>
@@ -7167,7 +7176,7 @@
       </c>
       <c r="C132" s="18"/>
       <c r="D132" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E132" s="18"/>
       <c r="F132" s="17" t="s">
@@ -7175,7 +7184,7 @@
       </c>
       <c r="G132" s="18"/>
       <c r="H132" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I132" s="18"/>
       <c r="J132" s="7"/>
@@ -7204,23 +7213,23 @@
         <v>111</v>
       </c>
       <c r="B134" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C134" s="18"/>
       <c r="D134" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E134" s="18"/>
       <c r="F134" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G134" s="18"/>
       <c r="H134" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I134" s="18"/>
       <c r="J134" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K134" s="7"/>
       <c r="L134" s="7"/>
@@ -7247,19 +7256,19 @@
         <v>112</v>
       </c>
       <c r="B136" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C136" s="18"/>
       <c r="D136" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E136" s="18"/>
       <c r="F136" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G136" s="18"/>
       <c r="H136" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I136" s="18"/>
       <c r="J136" s="7"/>
@@ -7273,19 +7282,19 @@
         <v>113</v>
       </c>
       <c r="B137" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C137" s="18"/>
       <c r="D137" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E137" s="18"/>
       <c r="F137" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G137" s="18"/>
       <c r="H137" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I137" s="18"/>
       <c r="J137" s="7"/>
@@ -7314,19 +7323,19 @@
         <v>114</v>
       </c>
       <c r="B139" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C139" s="18"/>
       <c r="D139" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E139" s="18"/>
       <c r="F139" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G139" s="18"/>
       <c r="H139" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I139" s="18"/>
       <c r="J139" s="7"/>
@@ -7340,19 +7349,19 @@
         <v>115</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C140" s="18"/>
       <c r="D140" s="17" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E140" s="18"/>
       <c r="F140" s="17" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G140" s="18"/>
       <c r="H140" s="17" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I140" s="18"/>
       <c r="J140" s="7"/>
@@ -7381,19 +7390,19 @@
         <v>116</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C142" s="18"/>
       <c r="D142" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E142" s="18"/>
       <c r="F142" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G142" s="18"/>
       <c r="H142" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I142" s="18"/>
       <c r="J142" s="7"/>
@@ -7407,19 +7416,19 @@
         <v>117</v>
       </c>
       <c r="B143" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C143" s="18"/>
       <c r="D143" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E143" s="18"/>
       <c r="F143" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G143" s="18"/>
       <c r="H143" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I143" s="18"/>
       <c r="J143" s="7"/>
@@ -7433,19 +7442,19 @@
         <v>118</v>
       </c>
       <c r="B144" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C144" s="18"/>
       <c r="D144" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E144" s="18"/>
       <c r="F144" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G144" s="18"/>
       <c r="H144" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I144" s="18"/>
       <c r="J144" s="7"/>
@@ -7459,19 +7468,19 @@
         <v>119</v>
       </c>
       <c r="B145" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C145" s="18"/>
       <c r="D145" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E145" s="18"/>
       <c r="F145" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G145" s="18"/>
       <c r="H145" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I145" s="18"/>
       <c r="J145" s="7"/>
@@ -7485,19 +7494,19 @@
         <v>120</v>
       </c>
       <c r="B146" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C146" s="18"/>
       <c r="D146" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E146" s="18"/>
       <c r="F146" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G146" s="18"/>
       <c r="H146" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I146" s="18"/>
       <c r="J146" s="7"/>
@@ -7511,19 +7520,19 @@
         <v>121</v>
       </c>
       <c r="B147" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C147" s="18"/>
       <c r="D147" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E147" s="18"/>
       <c r="F147" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G147" s="18"/>
       <c r="H147" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I147" s="18"/>
       <c r="J147" s="7"/>
@@ -7537,19 +7546,19 @@
         <v>122</v>
       </c>
       <c r="B148" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C148" s="18"/>
       <c r="D148" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E148" s="18"/>
       <c r="F148" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G148" s="18"/>
       <c r="H148" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I148" s="18"/>
       <c r="J148" s="7"/>
@@ -7563,19 +7572,19 @@
         <v>123</v>
       </c>
       <c r="B149" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C149" s="18"/>
       <c r="D149" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E149" s="18"/>
       <c r="F149" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G149" s="18"/>
       <c r="H149" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I149" s="18"/>
       <c r="J149" s="7"/>
@@ -7589,19 +7598,19 @@
         <v>123</v>
       </c>
       <c r="B150" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C150" s="18"/>
       <c r="D150" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E150" s="18"/>
       <c r="F150" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G150" s="18"/>
       <c r="H150" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I150" s="18"/>
       <c r="J150" s="7"/>
@@ -7615,19 +7624,19 @@
         <v>123</v>
       </c>
       <c r="B151" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C151" s="18"/>
       <c r="D151" s="17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E151" s="18"/>
       <c r="F151" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G151" s="18"/>
       <c r="H151" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I151" s="18"/>
       <c r="J151" s="7"/>
@@ -7641,19 +7650,19 @@
         <v>124</v>
       </c>
       <c r="B152" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C152" s="18"/>
       <c r="D152" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E152" s="18"/>
       <c r="F152" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G152" s="18"/>
       <c r="H152" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I152" s="18"/>
       <c r="J152" s="7"/>
@@ -7682,19 +7691,19 @@
         <v>125</v>
       </c>
       <c r="B154" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C154" s="18"/>
       <c r="D154" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E154" s="18"/>
       <c r="F154" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G154" s="18"/>
       <c r="H154" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I154" s="18"/>
       <c r="J154" s="7"/>
@@ -7708,19 +7717,19 @@
         <v>126</v>
       </c>
       <c r="B155" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C155" s="18"/>
       <c r="D155" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E155" s="18"/>
       <c r="F155" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G155" s="18"/>
       <c r="H155" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I155" s="18"/>
       <c r="J155" s="7"/>
@@ -7734,23 +7743,23 @@
         <v>127</v>
       </c>
       <c r="B156" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C156" s="18"/>
       <c r="D156" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E156" s="18"/>
       <c r="F156" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G156" s="18"/>
       <c r="H156" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I156" s="18"/>
       <c r="J156" s="7" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K156" s="7"/>
       <c r="L156" s="7"/>
@@ -7762,19 +7771,19 @@
         <v>128</v>
       </c>
       <c r="B157" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C157" s="18"/>
       <c r="D157" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E157" s="18"/>
       <c r="F157" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G157" s="18"/>
       <c r="H157" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I157" s="18"/>
       <c r="J157" s="7"/>
@@ -7788,19 +7797,19 @@
         <v>129</v>
       </c>
       <c r="B158" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C158" s="18"/>
       <c r="D158" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E158" s="18"/>
       <c r="F158" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G158" s="18"/>
       <c r="H158" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I158" s="18"/>
       <c r="J158" s="7"/>
@@ -7829,19 +7838,19 @@
         <v>130</v>
       </c>
       <c r="B160" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C160" s="18"/>
       <c r="D160" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E160" s="18"/>
       <c r="F160" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G160" s="18"/>
       <c r="H160" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I160" s="18"/>
       <c r="J160" s="7"/>
@@ -7855,19 +7864,19 @@
         <v>131</v>
       </c>
       <c r="B161" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C161" s="18"/>
       <c r="D161" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E161" s="18"/>
       <c r="F161" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G161" s="18"/>
       <c r="H161" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I161" s="18"/>
       <c r="J161" s="7"/>
@@ -7896,19 +7905,19 @@
         <v>132</v>
       </c>
       <c r="B163" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C163" s="18"/>
       <c r="D163" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E163" s="18"/>
       <c r="F163" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G163" s="18"/>
       <c r="H163" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I163" s="18"/>
       <c r="J163" s="7"/>
@@ -7922,19 +7931,19 @@
         <v>133</v>
       </c>
       <c r="B164" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C164" s="18"/>
       <c r="D164" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E164" s="18"/>
       <c r="F164" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G164" s="18"/>
       <c r="H164" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I164" s="18"/>
       <c r="J164" s="7"/>
@@ -7963,19 +7972,19 @@
         <v>134</v>
       </c>
       <c r="B166" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C166" s="18"/>
       <c r="D166" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E166" s="18"/>
       <c r="F166" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G166" s="18"/>
       <c r="H166" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I166" s="18"/>
       <c r="J166" s="7"/>
@@ -7989,19 +7998,19 @@
         <v>135</v>
       </c>
       <c r="B167" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C167" s="18"/>
       <c r="D167" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E167" s="18"/>
       <c r="F167" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G167" s="18"/>
       <c r="H167" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I167" s="18"/>
       <c r="J167" s="7"/>
@@ -8015,19 +8024,19 @@
         <v>136</v>
       </c>
       <c r="B168" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C168" s="18"/>
       <c r="D168" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E168" s="18"/>
       <c r="F168" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G168" s="18"/>
       <c r="H168" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I168" s="18"/>
       <c r="J168" s="7"/>
@@ -8041,19 +8050,19 @@
         <v>137</v>
       </c>
       <c r="B169" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C169" s="18"/>
       <c r="D169" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E169" s="25"/>
       <c r="F169" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G169" s="18"/>
       <c r="H169" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I169" s="18"/>
       <c r="J169" s="7"/>
@@ -8082,19 +8091,19 @@
         <v>138</v>
       </c>
       <c r="B171" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C171" s="18"/>
       <c r="D171" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E171" s="18"/>
       <c r="F171" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G171" s="18"/>
       <c r="H171" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I171" s="18"/>
       <c r="J171" s="7"/>
@@ -8123,19 +8132,19 @@
         <v>139</v>
       </c>
       <c r="B173" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C173" s="18"/>
       <c r="D173" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E173" s="25"/>
       <c r="F173" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G173" s="18"/>
       <c r="H173" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I173" s="18"/>
       <c r="J173" s="7"/>
@@ -8164,19 +8173,19 @@
         <v>140</v>
       </c>
       <c r="B175" s="17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C175" s="18"/>
       <c r="D175" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E175" s="18"/>
       <c r="F175" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G175" s="18"/>
       <c r="H175" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I175" s="18"/>
       <c r="J175" s="7"/>
@@ -8205,19 +8214,19 @@
         <v>141</v>
       </c>
       <c r="B177" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C177" s="18"/>
       <c r="D177" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E177" s="18"/>
       <c r="F177" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G177" s="18"/>
       <c r="H177" s="17" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I177" s="18"/>
       <c r="J177" s="7"/>
@@ -8241,82 +8250,77 @@
       <c r="M178" s="6"/>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A179" s="32"/>
-      <c r="B179" s="32"/>
-      <c r="C179" s="32"/>
-      <c r="D179" s="32"/>
-      <c r="E179" s="32"/>
-      <c r="F179" s="32"/>
-      <c r="G179" s="32"/>
-      <c r="H179" s="32"/>
-      <c r="I179" s="32"/>
-      <c r="J179" s="32"/>
-      <c r="K179" s="32"/>
-      <c r="L179" s="32"/>
-      <c r="M179" s="32"/>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A180" s="2">
+      <c r="A179" s="2">
         <f>A177+1</f>
         <v>142</v>
       </c>
-      <c r="B180" s="17" t="s">
-        <v>430</v>
-      </c>
-      <c r="C180" s="18"/>
-      <c r="D180" s="17"/>
-      <c r="E180" s="18"/>
-      <c r="F180" s="17" t="s">
-        <v>427</v>
-      </c>
-      <c r="G180" s="18"/>
-      <c r="H180" s="17" t="s">
-        <v>428</v>
-      </c>
-      <c r="I180" s="18"/>
-      <c r="J180" s="7"/>
-      <c r="K180" s="7"/>
-      <c r="L180" s="7"/>
-      <c r="M180" s="7"/>
+      <c r="B179" s="17" t="s">
+        <v>454</v>
+      </c>
+      <c r="C179" s="18"/>
+      <c r="D179" s="17"/>
+      <c r="E179" s="18"/>
+      <c r="F179" s="17" t="s">
+        <v>452</v>
+      </c>
+      <c r="G179" s="18"/>
+      <c r="H179" s="17" t="s">
+        <v>453</v>
+      </c>
+      <c r="I179" s="18"/>
+      <c r="J179" s="7"/>
+      <c r="K179" s="7"/>
+      <c r="L179" s="7"/>
+      <c r="M179" s="7"/>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A180" s="3"/>
+      <c r="B180" s="5"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="6"/>
+      <c r="F180" s="5"/>
+      <c r="G180" s="6"/>
+      <c r="H180" s="5"/>
+      <c r="I180" s="6"/>
+      <c r="J180" s="5"/>
+      <c r="K180" s="6"/>
+      <c r="L180" s="5"/>
+      <c r="M180" s="6"/>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A181" s="2">
-        <f t="shared" ref="A181:A196" si="5">A180+1</f>
-        <v>143</v>
-      </c>
-      <c r="B181" s="17" t="s">
-        <v>430</v>
-      </c>
-      <c r="C181" s="18"/>
-      <c r="D181" s="17"/>
-      <c r="E181" s="18"/>
-      <c r="F181" s="17" t="s">
-        <v>431</v>
-      </c>
-      <c r="G181" s="18"/>
-      <c r="H181" s="17"/>
-      <c r="I181" s="18"/>
-      <c r="J181" s="7"/>
-      <c r="K181" s="7"/>
-      <c r="L181" s="7"/>
-      <c r="M181" s="7"/>
+      <c r="A181" s="32"/>
+      <c r="B181" s="32"/>
+      <c r="C181" s="32"/>
+      <c r="D181" s="32"/>
+      <c r="E181" s="32"/>
+      <c r="F181" s="32"/>
+      <c r="G181" s="32"/>
+      <c r="H181" s="32"/>
+      <c r="I181" s="32"/>
+      <c r="J181" s="32"/>
+      <c r="K181" s="32"/>
+      <c r="L181" s="32"/>
+      <c r="M181" s="32"/>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <f t="shared" si="5"/>
-        <v>144</v>
+        <f>A179+1</f>
+        <v>143</v>
       </c>
       <c r="B182" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C182" s="18"/>
       <c r="D182" s="17"/>
       <c r="E182" s="18"/>
       <c r="F182" s="17" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="G182" s="18"/>
-      <c r="H182" s="17"/>
+      <c r="H182" s="17" t="s">
+        <v>426</v>
+      </c>
       <c r="I182" s="18"/>
       <c r="J182" s="7"/>
       <c r="K182" s="7"/>
@@ -8325,17 +8329,17 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <f t="shared" si="5"/>
-        <v>145</v>
+        <f t="shared" ref="A183:A198" si="5">A182+1</f>
+        <v>144</v>
       </c>
       <c r="B183" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C183" s="18"/>
       <c r="D183" s="17"/>
       <c r="E183" s="18"/>
       <c r="F183" s="17" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="G183" s="18"/>
       <c r="H183" s="17"/>
@@ -8348,16 +8352,16 @@
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <f t="shared" si="5"/>
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B184" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C184" s="18"/>
       <c r="D184" s="17"/>
       <c r="E184" s="18"/>
       <c r="F184" s="17" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G184" s="18"/>
       <c r="H184" s="17"/>
@@ -8370,16 +8374,16 @@
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <f t="shared" si="5"/>
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B185" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C185" s="18"/>
       <c r="D185" s="17"/>
       <c r="E185" s="18"/>
       <c r="F185" s="17" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G185" s="18"/>
       <c r="H185" s="17"/>
@@ -8392,21 +8396,19 @@
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <f t="shared" si="5"/>
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B186" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C186" s="18"/>
       <c r="D186" s="17"/>
       <c r="E186" s="18"/>
       <c r="F186" s="17" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="G186" s="18"/>
-      <c r="H186" s="17" t="s">
-        <v>437</v>
-      </c>
+      <c r="H186" s="17"/>
       <c r="I186" s="18"/>
       <c r="J186" s="7"/>
       <c r="K186" s="7"/>
@@ -8416,25 +8418,21 @@
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <f t="shared" si="5"/>
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B187" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C187" s="18"/>
       <c r="D187" s="17"/>
       <c r="E187" s="18"/>
       <c r="F187" s="17" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="G187" s="18"/>
-      <c r="H187" s="17" t="s">
-        <v>443</v>
-      </c>
+      <c r="H187" s="17"/>
       <c r="I187" s="18"/>
-      <c r="J187" s="7" t="s">
-        <v>444</v>
-      </c>
+      <c r="J187" s="7"/>
       <c r="K187" s="7"/>
       <c r="L187" s="7"/>
       <c r="M187" s="7"/>
@@ -8442,20 +8440,20 @@
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <f t="shared" si="5"/>
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B188" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C188" s="18"/>
       <c r="D188" s="17"/>
       <c r="E188" s="18"/>
-      <c r="F188" s="31" t="s">
-        <v>445</v>
+      <c r="F188" s="17" t="s">
+        <v>434</v>
       </c>
       <c r="G188" s="18"/>
-      <c r="H188" s="31" t="s">
-        <v>446</v>
+      <c r="H188" s="17" t="s">
+        <v>435</v>
       </c>
       <c r="I188" s="18"/>
       <c r="J188" s="7"/>
@@ -8466,19 +8464,25 @@
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <f t="shared" si="5"/>
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B189" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C189" s="18"/>
       <c r="D189" s="17"/>
       <c r="E189" s="18"/>
-      <c r="F189" s="17"/>
+      <c r="F189" s="17" t="s">
+        <v>440</v>
+      </c>
       <c r="G189" s="18"/>
-      <c r="H189" s="17"/>
+      <c r="H189" s="17" t="s">
+        <v>441</v>
+      </c>
       <c r="I189" s="18"/>
-      <c r="J189" s="7"/>
+      <c r="J189" s="7" t="s">
+        <v>442</v>
+      </c>
       <c r="K189" s="7"/>
       <c r="L189" s="7"/>
       <c r="M189" s="7"/>
@@ -8486,17 +8490,21 @@
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <f t="shared" si="5"/>
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B190" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C190" s="18"/>
       <c r="D190" s="17"/>
       <c r="E190" s="18"/>
-      <c r="F190" s="17"/>
+      <c r="F190" s="31" t="s">
+        <v>443</v>
+      </c>
       <c r="G190" s="18"/>
-      <c r="H190" s="17"/>
+      <c r="H190" s="31" t="s">
+        <v>444</v>
+      </c>
       <c r="I190" s="18"/>
       <c r="J190" s="7"/>
       <c r="K190" s="7"/>
@@ -8506,10 +8514,10 @@
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <f t="shared" si="5"/>
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B191" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C191" s="18"/>
       <c r="D191" s="17"/>
@@ -8526,10 +8534,10 @@
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <f t="shared" si="5"/>
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B192" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C192" s="18"/>
       <c r="D192" s="17"/>
@@ -8546,10 +8554,10 @@
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B193" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C193" s="18"/>
       <c r="D193" s="17"/>
@@ -8566,10 +8574,10 @@
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <f t="shared" si="5"/>
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B194" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C194" s="18"/>
       <c r="D194" s="17"/>
@@ -8586,10 +8594,10 @@
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <f t="shared" si="5"/>
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B195" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C195" s="18"/>
       <c r="D195" s="17"/>
@@ -8606,10 +8614,10 @@
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <f t="shared" si="5"/>
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B196" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C196" s="18"/>
       <c r="D196" s="17"/>
@@ -8623,15 +8631,80 @@
       <c r="L196" s="7"/>
       <c r="M196" s="7"/>
     </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <f t="shared" si="5"/>
+        <v>158</v>
+      </c>
+      <c r="B197" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="C197" s="18"/>
+      <c r="D197" s="17"/>
+      <c r="E197" s="18"/>
+      <c r="F197" s="17"/>
+      <c r="G197" s="18"/>
+      <c r="H197" s="17"/>
+      <c r="I197" s="18"/>
+      <c r="J197" s="7"/>
+      <c r="K197" s="7"/>
+      <c r="L197" s="7"/>
+      <c r="M197" s="7"/>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <f t="shared" si="5"/>
+        <v>159</v>
+      </c>
+      <c r="B198" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="C198" s="18"/>
+      <c r="D198" s="17"/>
+      <c r="E198" s="18"/>
+      <c r="F198" s="17"/>
+      <c r="G198" s="18"/>
+      <c r="H198" s="17"/>
+      <c r="I198" s="18"/>
+      <c r="J198" s="7"/>
+      <c r="K198" s="7"/>
+      <c r="L198" s="7"/>
+      <c r="M198" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="1154">
+  <mergeCells count="1160">
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="D179:E179"/>
+    <mergeCell ref="F179:G179"/>
+    <mergeCell ref="H179:I179"/>
+    <mergeCell ref="J179:K179"/>
+    <mergeCell ref="L179:M179"/>
+    <mergeCell ref="B198:C198"/>
+    <mergeCell ref="D198:E198"/>
+    <mergeCell ref="F198:G198"/>
+    <mergeCell ref="H198:I198"/>
+    <mergeCell ref="J198:K198"/>
+    <mergeCell ref="L198:M198"/>
+    <mergeCell ref="A181:M181"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="D194:E194"/>
+    <mergeCell ref="F194:G194"/>
+    <mergeCell ref="H194:I194"/>
+    <mergeCell ref="J194:K194"/>
+    <mergeCell ref="L194:M194"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="D195:E195"/>
+    <mergeCell ref="F195:G195"/>
+    <mergeCell ref="H195:I195"/>
+    <mergeCell ref="J195:K195"/>
+    <mergeCell ref="L195:M195"/>
     <mergeCell ref="B196:C196"/>
     <mergeCell ref="D196:E196"/>
     <mergeCell ref="F196:G196"/>
     <mergeCell ref="H196:I196"/>
     <mergeCell ref="J196:K196"/>
     <mergeCell ref="L196:M196"/>
-    <mergeCell ref="A179:M179"/>
+    <mergeCell ref="B191:C191"/>
     <mergeCell ref="B192:C192"/>
     <mergeCell ref="D192:E192"/>
     <mergeCell ref="F192:G192"/>
@@ -8644,31 +8717,35 @@
     <mergeCell ref="H193:I193"/>
     <mergeCell ref="J193:K193"/>
     <mergeCell ref="L193:M193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="D194:E194"/>
-    <mergeCell ref="F194:G194"/>
-    <mergeCell ref="H194:I194"/>
-    <mergeCell ref="J194:K194"/>
-    <mergeCell ref="L194:M194"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="D197:E197"/>
+    <mergeCell ref="F197:G197"/>
+    <mergeCell ref="H197:I197"/>
+    <mergeCell ref="J197:K197"/>
+    <mergeCell ref="L197:M197"/>
     <mergeCell ref="B189:C189"/>
+    <mergeCell ref="D189:E189"/>
+    <mergeCell ref="F189:G189"/>
+    <mergeCell ref="H189:I189"/>
+    <mergeCell ref="J189:K189"/>
+    <mergeCell ref="L189:M189"/>
     <mergeCell ref="B190:C190"/>
     <mergeCell ref="D190:E190"/>
     <mergeCell ref="F190:G190"/>
     <mergeCell ref="H190:I190"/>
     <mergeCell ref="J190:K190"/>
     <mergeCell ref="L190:M190"/>
-    <mergeCell ref="B191:C191"/>
     <mergeCell ref="D191:E191"/>
     <mergeCell ref="F191:G191"/>
     <mergeCell ref="H191:I191"/>
     <mergeCell ref="J191:K191"/>
     <mergeCell ref="L191:M191"/>
-    <mergeCell ref="B195:C195"/>
-    <mergeCell ref="D195:E195"/>
-    <mergeCell ref="F195:G195"/>
-    <mergeCell ref="H195:I195"/>
-    <mergeCell ref="J195:K195"/>
-    <mergeCell ref="L195:M195"/>
+    <mergeCell ref="B186:C186"/>
+    <mergeCell ref="D186:E186"/>
+    <mergeCell ref="F186:G186"/>
+    <mergeCell ref="H186:I186"/>
+    <mergeCell ref="J186:K186"/>
+    <mergeCell ref="L186:M186"/>
     <mergeCell ref="B187:C187"/>
     <mergeCell ref="D187:E187"/>
     <mergeCell ref="F187:G187"/>
@@ -8681,11 +8758,13 @@
     <mergeCell ref="H188:I188"/>
     <mergeCell ref="J188:K188"/>
     <mergeCell ref="L188:M188"/>
-    <mergeCell ref="D189:E189"/>
-    <mergeCell ref="F189:G189"/>
-    <mergeCell ref="H189:I189"/>
-    <mergeCell ref="J189:K189"/>
-    <mergeCell ref="L189:M189"/>
+    <mergeCell ref="L182:M182"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="D183:E183"/>
+    <mergeCell ref="F183:G183"/>
+    <mergeCell ref="H183:I183"/>
+    <mergeCell ref="J183:K183"/>
+    <mergeCell ref="L183:M183"/>
     <mergeCell ref="B184:C184"/>
     <mergeCell ref="D184:E184"/>
     <mergeCell ref="F184:G184"/>
@@ -8698,36 +8777,11 @@
     <mergeCell ref="H185:I185"/>
     <mergeCell ref="J185:K185"/>
     <mergeCell ref="L185:M185"/>
-    <mergeCell ref="B186:C186"/>
-    <mergeCell ref="D186:E186"/>
-    <mergeCell ref="F186:G186"/>
-    <mergeCell ref="H186:I186"/>
-    <mergeCell ref="J186:K186"/>
-    <mergeCell ref="L186:M186"/>
-    <mergeCell ref="L180:M180"/>
-    <mergeCell ref="B181:C181"/>
-    <mergeCell ref="D181:E181"/>
-    <mergeCell ref="F181:G181"/>
-    <mergeCell ref="H181:I181"/>
-    <mergeCell ref="J181:K181"/>
-    <mergeCell ref="L181:M181"/>
     <mergeCell ref="B182:C182"/>
     <mergeCell ref="D182:E182"/>
     <mergeCell ref="F182:G182"/>
     <mergeCell ref="H182:I182"/>
     <mergeCell ref="J182:K182"/>
-    <mergeCell ref="L182:M182"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="D183:E183"/>
-    <mergeCell ref="F183:G183"/>
-    <mergeCell ref="H183:I183"/>
-    <mergeCell ref="J183:K183"/>
-    <mergeCell ref="L183:M183"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="D180:E180"/>
-    <mergeCell ref="F180:G180"/>
-    <mergeCell ref="H180:I180"/>
-    <mergeCell ref="J180:K180"/>
     <mergeCell ref="F139:G139"/>
     <mergeCell ref="H139:I139"/>
     <mergeCell ref="J139:K139"/>
@@ -8846,6 +8900,16 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="F132:G132"/>
     <mergeCell ref="F136:G136"/>
     <mergeCell ref="F70:G70"/>
@@ -8876,20 +8940,8 @@
     <mergeCell ref="B96:C96"/>
     <mergeCell ref="B109:C109"/>
     <mergeCell ref="F125:G125"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="F134:G134"/>
     <mergeCell ref="D84:E84"/>
     <mergeCell ref="F130:G130"/>
     <mergeCell ref="D50:E50"/>
@@ -8899,10 +8951,19 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="D56:E56"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="F120:G120"/>
+    <mergeCell ref="H120:I120"/>
+    <mergeCell ref="H83:I83"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
@@ -8925,6 +8986,16 @@
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="H77:I77"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="F2:G3"/>
@@ -8949,22 +9020,7 @@
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="H43:I43"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="H84:I84"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="H32:I32"/>
@@ -8972,15 +9028,6 @@
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="F42:G42"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H38:I38"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="H29:I29"/>
@@ -9007,9 +9054,12 @@
     <mergeCell ref="F53:G53"/>
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="B51:C51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H74:I74"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="B82:C82"/>
@@ -9031,6 +9081,17 @@
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="F49:G49"/>
@@ -9255,7 +9316,6 @@
     <mergeCell ref="J53:K53"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="J34:K34"/>
-    <mergeCell ref="H111:I111"/>
     <mergeCell ref="J172:K172"/>
     <mergeCell ref="J173:K173"/>
     <mergeCell ref="J174:K174"/>
@@ -9312,7 +9372,6 @@
     <mergeCell ref="D148:E148"/>
     <mergeCell ref="D149:E149"/>
     <mergeCell ref="B134:C134"/>
-    <mergeCell ref="F134:G134"/>
     <mergeCell ref="H134:I134"/>
     <mergeCell ref="B124:C124"/>
     <mergeCell ref="H137:I137"/>
@@ -9377,9 +9436,6 @@
     <mergeCell ref="H119:I119"/>
     <mergeCell ref="J119:K119"/>
     <mergeCell ref="B120:C120"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="F120:G120"/>
-    <mergeCell ref="H120:I120"/>
     <mergeCell ref="J120:K120"/>
     <mergeCell ref="J111:K111"/>
     <mergeCell ref="J113:K113"/>
@@ -9412,9 +9468,6 @@
     <mergeCell ref="H81:I81"/>
     <mergeCell ref="H80:I80"/>
     <mergeCell ref="H79:I79"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F73:G73"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:E23"/>
@@ -9543,6 +9596,7 @@
     <mergeCell ref="J96:K96"/>
     <mergeCell ref="F93:G93"/>
     <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H93:I93"/>
     <mergeCell ref="J84:K84"/>
     <mergeCell ref="F82:G82"/>
     <mergeCell ref="H82:I82"/>

</xml_diff>